<commit_message>
complete costeffectiveness_tree print method
</commit_message>
<xml_diff>
--- a/data/scenario-parameter-values.xlsx
+++ b/data/scenario-parameter-values.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="11025" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="11025" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="details" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="15">
   <si>
     <t>project: LTBI screening</t>
   </si>
@@ -54,6 +54,21 @@
   </si>
   <si>
     <t>Not Agree to Screen</t>
+  </si>
+  <si>
+    <t>node</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>distn</t>
+  </si>
+  <si>
+    <t>unif</t>
   </si>
 </sst>
 </file>
@@ -103,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -112,6 +127,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -385,7 +405,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -441,1464 +461,3095 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B181"/>
+  <dimension ref="A1:E181"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9">
+        <v>50</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>20</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>20</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22">
+        <v>50</v>
+      </c>
+      <c r="D22">
+        <v>50</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23">
+        <v>50</v>
+      </c>
+      <c r="D23">
+        <v>50</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24">
+        <v>50</v>
+      </c>
+      <c r="D24">
+        <v>50</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>50</v>
+      </c>
+      <c r="D25">
+        <v>50</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26">
+        <v>50</v>
+      </c>
+      <c r="D26">
+        <v>50</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27">
+        <v>100</v>
+      </c>
+      <c r="D27">
+        <v>100</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28">
+        <v>100</v>
+      </c>
+      <c r="D28">
+        <v>100</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>100</v>
+      </c>
+      <c r="D29">
+        <v>100</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30">
+        <v>100</v>
+      </c>
+      <c r="D30">
+        <v>100</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>100</v>
+      </c>
+      <c r="D31">
+        <v>100</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <v>20</v>
+      </c>
+      <c r="D32">
+        <v>20</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>20</v>
+      </c>
+      <c r="D33">
+        <v>20</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34">
+        <v>20</v>
+      </c>
+      <c r="D34">
+        <v>20</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35">
+        <v>20</v>
+      </c>
+      <c r="D35">
+        <v>20</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36">
+        <v>20</v>
+      </c>
+      <c r="D36">
+        <v>20</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37">
+        <v>50</v>
+      </c>
+      <c r="D37">
+        <v>50</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38">
+        <v>50</v>
+      </c>
+      <c r="D38">
+        <v>50</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39">
+        <v>50</v>
+      </c>
+      <c r="D39">
+        <v>50</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40">
+        <v>50</v>
+      </c>
+      <c r="D40">
+        <v>50</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41">
+        <v>50</v>
+      </c>
+      <c r="D41">
+        <v>50</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42">
+        <v>100</v>
+      </c>
+      <c r="D42">
+        <v>100</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43">
+        <v>100</v>
+      </c>
+      <c r="D43">
+        <v>100</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44">
+        <v>100</v>
+      </c>
+      <c r="D44">
+        <v>100</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45">
+        <v>100</v>
+      </c>
+      <c r="D45">
+        <v>100</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46">
+        <v>100</v>
+      </c>
+      <c r="D46">
+        <v>100</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47">
+        <v>20</v>
+      </c>
+      <c r="D47">
+        <v>20</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48">
+        <v>20</v>
+      </c>
+      <c r="D48">
+        <v>20</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49">
+        <v>20</v>
+      </c>
+      <c r="D49">
+        <v>20</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50">
+        <v>20</v>
+      </c>
+      <c r="D50">
+        <v>20</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51">
+        <v>20</v>
+      </c>
+      <c r="D51">
+        <v>20</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52">
+        <v>50</v>
+      </c>
+      <c r="D52">
+        <v>50</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53">
+        <v>50</v>
+      </c>
+      <c r="D53">
+        <v>50</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54">
+        <v>50</v>
+      </c>
+      <c r="D54">
+        <v>50</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55">
+        <v>50</v>
+      </c>
+      <c r="D55">
+        <v>50</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56">
+        <v>50</v>
+      </c>
+      <c r="D56">
+        <v>50</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57">
+        <v>100</v>
+      </c>
+      <c r="D57">
+        <v>100</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58">
+        <v>100</v>
+      </c>
+      <c r="D58">
+        <v>100</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59">
+        <v>100</v>
+      </c>
+      <c r="D59">
+        <v>100</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60">
+        <v>100</v>
+      </c>
+      <c r="D60">
+        <v>100</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61">
+        <v>100</v>
+      </c>
+      <c r="D61">
+        <v>100</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62">
+        <v>20</v>
+      </c>
+      <c r="D62">
+        <v>20</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63">
+        <v>20</v>
+      </c>
+      <c r="D63">
+        <v>20</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
-      <c r="B64">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64">
+        <v>20</v>
+      </c>
+      <c r="D64">
+        <v>20</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65">
+        <v>20</v>
+      </c>
+      <c r="D65">
+        <v>20</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
-      <c r="B66">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66">
+        <v>20</v>
+      </c>
+      <c r="D66">
+        <v>20</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
-      <c r="B67">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67">
+        <v>50</v>
+      </c>
+      <c r="D67">
+        <v>50</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
-      <c r="B68">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68">
+        <v>50</v>
+      </c>
+      <c r="D68">
+        <v>50</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
-      <c r="B69">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69">
+        <v>50</v>
+      </c>
+      <c r="D69">
+        <v>50</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
-      <c r="B70">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70">
+        <v>50</v>
+      </c>
+      <c r="D70">
+        <v>50</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
-      <c r="B71">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71">
+        <v>50</v>
+      </c>
+      <c r="D71">
+        <v>50</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
-      <c r="B72">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72">
+        <v>100</v>
+      </c>
+      <c r="D72">
+        <v>100</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
-      <c r="B73">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73">
+        <v>100</v>
+      </c>
+      <c r="D73">
+        <v>100</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
-      <c r="B74">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74">
+        <v>100</v>
+      </c>
+      <c r="D74">
+        <v>100</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
-      <c r="B75">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75">
+        <v>100</v>
+      </c>
+      <c r="D75">
+        <v>100</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
-      <c r="B76">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>14</v>
+      </c>
+      <c r="C76">
+        <v>100</v>
+      </c>
+      <c r="D76">
+        <v>100</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
-      <c r="B77">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>14</v>
+      </c>
+      <c r="C77">
+        <v>20</v>
+      </c>
+      <c r="D77">
+        <v>20</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
-      <c r="B78">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>14</v>
+      </c>
+      <c r="C78">
+        <v>20</v>
+      </c>
+      <c r="D78">
+        <v>20</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
-      <c r="B79">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>14</v>
+      </c>
+      <c r="C79">
+        <v>20</v>
+      </c>
+      <c r="D79">
+        <v>20</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
-      <c r="B80">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>14</v>
+      </c>
+      <c r="C80">
+        <v>20</v>
+      </c>
+      <c r="D80">
+        <v>20</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
-      <c r="B81">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>14</v>
+      </c>
+      <c r="C81">
+        <v>20</v>
+      </c>
+      <c r="D81">
+        <v>20</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
-      <c r="B82">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>14</v>
+      </c>
+      <c r="C82">
+        <v>50</v>
+      </c>
+      <c r="D82">
+        <v>50</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
-      <c r="B83">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83">
+        <v>50</v>
+      </c>
+      <c r="D83">
+        <v>50</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
-      <c r="B84">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84">
+        <v>50</v>
+      </c>
+      <c r="D84">
+        <v>50</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
-      <c r="B85">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>14</v>
+      </c>
+      <c r="C85">
+        <v>50</v>
+      </c>
+      <c r="D85">
+        <v>50</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
-      <c r="B86">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>14</v>
+      </c>
+      <c r="C86">
+        <v>50</v>
+      </c>
+      <c r="D86">
+        <v>50</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
-      <c r="B87">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87">
+        <v>100</v>
+      </c>
+      <c r="D87">
+        <v>100</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
-      <c r="B88">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88">
+        <v>100</v>
+      </c>
+      <c r="D88">
+        <v>100</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
-      <c r="B89">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89">
+        <v>100</v>
+      </c>
+      <c r="D89">
+        <v>100</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
-      <c r="B90">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90">
+        <v>100</v>
+      </c>
+      <c r="D90">
+        <v>100</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
-      <c r="B91">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>14</v>
+      </c>
+      <c r="C91">
+        <v>100</v>
+      </c>
+      <c r="D91">
+        <v>100</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
-      <c r="B92">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>14</v>
+      </c>
+      <c r="C92">
+        <v>20</v>
+      </c>
+      <c r="D92">
+        <v>20</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
-      <c r="B93">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93">
+        <v>20</v>
+      </c>
+      <c r="D93">
+        <v>20</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
-      <c r="B94">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>14</v>
+      </c>
+      <c r="C94">
+        <v>20</v>
+      </c>
+      <c r="D94">
+        <v>20</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
-      <c r="B95">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>14</v>
+      </c>
+      <c r="C95">
+        <v>20</v>
+      </c>
+      <c r="D95">
+        <v>20</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
-      <c r="B96">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>14</v>
+      </c>
+      <c r="C96">
+        <v>20</v>
+      </c>
+      <c r="D96">
+        <v>20</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
-      <c r="B97">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>14</v>
+      </c>
+      <c r="C97">
+        <v>50</v>
+      </c>
+      <c r="D97">
+        <v>50</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
-      <c r="B98">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>14</v>
+      </c>
+      <c r="C98">
+        <v>50</v>
+      </c>
+      <c r="D98">
+        <v>50</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
-      <c r="B99">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>14</v>
+      </c>
+      <c r="C99">
+        <v>50</v>
+      </c>
+      <c r="D99">
+        <v>50</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
-      <c r="B100">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>14</v>
+      </c>
+      <c r="C100">
+        <v>50</v>
+      </c>
+      <c r="D100">
+        <v>50</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
-      <c r="B101">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>14</v>
+      </c>
+      <c r="C101">
+        <v>50</v>
+      </c>
+      <c r="D101">
+        <v>50</v>
+      </c>
+      <c r="E101" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
-      <c r="B102">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>14</v>
+      </c>
+      <c r="C102">
+        <v>100</v>
+      </c>
+      <c r="D102">
+        <v>100</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
-      <c r="B103">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>14</v>
+      </c>
+      <c r="C103">
+        <v>100</v>
+      </c>
+      <c r="D103">
+        <v>100</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
-      <c r="B104">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>14</v>
+      </c>
+      <c r="C104">
+        <v>100</v>
+      </c>
+      <c r="D104">
+        <v>100</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
-      <c r="B105">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>14</v>
+      </c>
+      <c r="C105">
+        <v>100</v>
+      </c>
+      <c r="D105">
+        <v>100</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
-      <c r="B106">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>14</v>
+      </c>
+      <c r="C106">
+        <v>100</v>
+      </c>
+      <c r="D106">
+        <v>100</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
-      <c r="B107">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>14</v>
+      </c>
+      <c r="C107">
+        <v>20</v>
+      </c>
+      <c r="D107">
+        <v>20</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
-      <c r="B108">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>14</v>
+      </c>
+      <c r="C108">
+        <v>20</v>
+      </c>
+      <c r="D108">
+        <v>20</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
-      <c r="B109">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>14</v>
+      </c>
+      <c r="C109">
+        <v>20</v>
+      </c>
+      <c r="D109">
+        <v>20</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
-      <c r="B110">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>14</v>
+      </c>
+      <c r="C110">
+        <v>20</v>
+      </c>
+      <c r="D110">
+        <v>20</v>
+      </c>
+      <c r="E110" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
-      <c r="B111">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>14</v>
+      </c>
+      <c r="C111">
+        <v>20</v>
+      </c>
+      <c r="D111">
+        <v>20</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
-      <c r="B112">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>14</v>
+      </c>
+      <c r="C112">
+        <v>50</v>
+      </c>
+      <c r="D112">
+        <v>50</v>
+      </c>
+      <c r="E112" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
-      <c r="B113">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>14</v>
+      </c>
+      <c r="C113">
+        <v>50</v>
+      </c>
+      <c r="D113">
+        <v>50</v>
+      </c>
+      <c r="E113" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
-      <c r="B114">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>14</v>
+      </c>
+      <c r="C114">
+        <v>50</v>
+      </c>
+      <c r="D114">
+        <v>50</v>
+      </c>
+      <c r="E114" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
-      <c r="B115">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>14</v>
+      </c>
+      <c r="C115">
+        <v>50</v>
+      </c>
+      <c r="D115">
+        <v>50</v>
+      </c>
+      <c r="E115" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
-      <c r="B116">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>14</v>
+      </c>
+      <c r="C116">
+        <v>50</v>
+      </c>
+      <c r="D116">
+        <v>50</v>
+      </c>
+      <c r="E116" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
-      <c r="B117">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>14</v>
+      </c>
+      <c r="C117">
+        <v>100</v>
+      </c>
+      <c r="D117">
+        <v>100</v>
+      </c>
+      <c r="E117" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
-      <c r="B118">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>14</v>
+      </c>
+      <c r="C118">
+        <v>100</v>
+      </c>
+      <c r="D118">
+        <v>100</v>
+      </c>
+      <c r="E118" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
-      <c r="B119">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>14</v>
+      </c>
+      <c r="C119">
+        <v>100</v>
+      </c>
+      <c r="D119">
+        <v>100</v>
+      </c>
+      <c r="E119" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
-      <c r="B120">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>14</v>
+      </c>
+      <c r="C120">
+        <v>100</v>
+      </c>
+      <c r="D120">
+        <v>100</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
-      <c r="B121">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>14</v>
+      </c>
+      <c r="C121">
+        <v>100</v>
+      </c>
+      <c r="D121">
+        <v>100</v>
+      </c>
+      <c r="E121" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
-      <c r="B122">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>14</v>
+      </c>
+      <c r="C122">
+        <v>20</v>
+      </c>
+      <c r="D122">
+        <v>20</v>
+      </c>
+      <c r="E122" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
-      <c r="B123">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>14</v>
+      </c>
+      <c r="C123">
+        <v>20</v>
+      </c>
+      <c r="D123">
+        <v>20</v>
+      </c>
+      <c r="E123" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
-      <c r="B124">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>14</v>
+      </c>
+      <c r="C124">
+        <v>20</v>
+      </c>
+      <c r="D124">
+        <v>20</v>
+      </c>
+      <c r="E124" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
-      <c r="B125">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>14</v>
+      </c>
+      <c r="C125">
+        <v>20</v>
+      </c>
+      <c r="D125">
+        <v>20</v>
+      </c>
+      <c r="E125" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
-      <c r="B126">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>14</v>
+      </c>
+      <c r="C126">
+        <v>20</v>
+      </c>
+      <c r="D126">
+        <v>20</v>
+      </c>
+      <c r="E126" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
-      <c r="B127">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>14</v>
+      </c>
+      <c r="C127">
+        <v>50</v>
+      </c>
+      <c r="D127">
+        <v>50</v>
+      </c>
+      <c r="E127" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
-      <c r="B128">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>14</v>
+      </c>
+      <c r="C128">
+        <v>50</v>
+      </c>
+      <c r="D128">
+        <v>50</v>
+      </c>
+      <c r="E128" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
-      <c r="B129">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>14</v>
+      </c>
+      <c r="C129">
+        <v>50</v>
+      </c>
+      <c r="D129">
+        <v>50</v>
+      </c>
+      <c r="E129" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
-      <c r="B130">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>14</v>
+      </c>
+      <c r="C130">
+        <v>50</v>
+      </c>
+      <c r="D130">
+        <v>50</v>
+      </c>
+      <c r="E130" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
-      <c r="B131">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>14</v>
+      </c>
+      <c r="C131">
+        <v>50</v>
+      </c>
+      <c r="D131">
+        <v>50</v>
+      </c>
+      <c r="E131" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
-      <c r="B132">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>14</v>
+      </c>
+      <c r="C132">
+        <v>100</v>
+      </c>
+      <c r="D132">
+        <v>100</v>
+      </c>
+      <c r="E132" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
-      <c r="B133">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>14</v>
+      </c>
+      <c r="C133">
+        <v>100</v>
+      </c>
+      <c r="D133">
+        <v>100</v>
+      </c>
+      <c r="E133" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
-      <c r="B134">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>14</v>
+      </c>
+      <c r="C134">
+        <v>100</v>
+      </c>
+      <c r="D134">
+        <v>100</v>
+      </c>
+      <c r="E134" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
-      <c r="B135">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>14</v>
+      </c>
+      <c r="C135">
+        <v>100</v>
+      </c>
+      <c r="D135">
+        <v>100</v>
+      </c>
+      <c r="E135" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
-      <c r="B136">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>14</v>
+      </c>
+      <c r="C136">
+        <v>100</v>
+      </c>
+      <c r="D136">
+        <v>100</v>
+      </c>
+      <c r="E136" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
-      <c r="B137">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>14</v>
+      </c>
+      <c r="C137">
+        <v>20</v>
+      </c>
+      <c r="D137">
+        <v>20</v>
+      </c>
+      <c r="E137" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
-      <c r="B138">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>14</v>
+      </c>
+      <c r="C138">
+        <v>20</v>
+      </c>
+      <c r="D138">
+        <v>20</v>
+      </c>
+      <c r="E138" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
-      <c r="B139">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>14</v>
+      </c>
+      <c r="C139">
+        <v>20</v>
+      </c>
+      <c r="D139">
+        <v>20</v>
+      </c>
+      <c r="E139" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
-      <c r="B140">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>14</v>
+      </c>
+      <c r="C140">
+        <v>20</v>
+      </c>
+      <c r="D140">
+        <v>20</v>
+      </c>
+      <c r="E140" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
-      <c r="B141">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>14</v>
+      </c>
+      <c r="C141">
+        <v>20</v>
+      </c>
+      <c r="D141">
+        <v>20</v>
+      </c>
+      <c r="E141" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
-      <c r="B142">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>14</v>
+      </c>
+      <c r="C142">
+        <v>50</v>
+      </c>
+      <c r="D142">
+        <v>50</v>
+      </c>
+      <c r="E142" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
-      <c r="B143">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>14</v>
+      </c>
+      <c r="C143">
+        <v>50</v>
+      </c>
+      <c r="D143">
+        <v>50</v>
+      </c>
+      <c r="E143" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
-      <c r="B144">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>14</v>
+      </c>
+      <c r="C144">
+        <v>50</v>
+      </c>
+      <c r="D144">
+        <v>50</v>
+      </c>
+      <c r="E144" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
-      <c r="B145">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>14</v>
+      </c>
+      <c r="C145">
+        <v>50</v>
+      </c>
+      <c r="D145">
+        <v>50</v>
+      </c>
+      <c r="E145" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
-      <c r="B146">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>14</v>
+      </c>
+      <c r="C146">
+        <v>50</v>
+      </c>
+      <c r="D146">
+        <v>50</v>
+      </c>
+      <c r="E146" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
-      <c r="B147">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>14</v>
+      </c>
+      <c r="C147">
+        <v>100</v>
+      </c>
+      <c r="D147">
+        <v>100</v>
+      </c>
+      <c r="E147" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
-      <c r="B148">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>14</v>
+      </c>
+      <c r="C148">
+        <v>100</v>
+      </c>
+      <c r="D148">
+        <v>100</v>
+      </c>
+      <c r="E148" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
-      <c r="B149">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>14</v>
+      </c>
+      <c r="C149">
+        <v>100</v>
+      </c>
+      <c r="D149">
+        <v>100</v>
+      </c>
+      <c r="E149" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
-      <c r="B150">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>14</v>
+      </c>
+      <c r="C150">
+        <v>100</v>
+      </c>
+      <c r="D150">
+        <v>100</v>
+      </c>
+      <c r="E150" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
-      <c r="B151">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>14</v>
+      </c>
+      <c r="C151">
+        <v>100</v>
+      </c>
+      <c r="D151">
+        <v>100</v>
+      </c>
+      <c r="E151" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
-      <c r="B152">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>14</v>
+      </c>
+      <c r="C152">
+        <v>20</v>
+      </c>
+      <c r="D152">
+        <v>20</v>
+      </c>
+      <c r="E152" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
-      <c r="B153">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>14</v>
+      </c>
+      <c r="C153">
+        <v>20</v>
+      </c>
+      <c r="D153">
+        <v>20</v>
+      </c>
+      <c r="E153" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
-      <c r="B154">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>14</v>
+      </c>
+      <c r="C154">
+        <v>20</v>
+      </c>
+      <c r="D154">
+        <v>20</v>
+      </c>
+      <c r="E154" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
-      <c r="B155">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
+        <v>14</v>
+      </c>
+      <c r="C155">
+        <v>20</v>
+      </c>
+      <c r="D155">
+        <v>20</v>
+      </c>
+      <c r="E155" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
-      <c r="B156">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
+        <v>14</v>
+      </c>
+      <c r="C156">
+        <v>20</v>
+      </c>
+      <c r="D156">
+        <v>20</v>
+      </c>
+      <c r="E156" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
-      <c r="B157">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>14</v>
+      </c>
+      <c r="C157">
+        <v>50</v>
+      </c>
+      <c r="D157">
+        <v>50</v>
+      </c>
+      <c r="E157" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
-      <c r="B158">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>14</v>
+      </c>
+      <c r="C158">
+        <v>50</v>
+      </c>
+      <c r="D158">
+        <v>50</v>
+      </c>
+      <c r="E158" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
-      <c r="B159">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>14</v>
+      </c>
+      <c r="C159">
+        <v>50</v>
+      </c>
+      <c r="D159">
+        <v>50</v>
+      </c>
+      <c r="E159" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
-      <c r="B160">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
+        <v>14</v>
+      </c>
+      <c r="C160">
+        <v>50</v>
+      </c>
+      <c r="D160">
+        <v>50</v>
+      </c>
+      <c r="E160" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
-      <c r="B161">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>14</v>
+      </c>
+      <c r="C161">
+        <v>50</v>
+      </c>
+      <c r="D161">
+        <v>50</v>
+      </c>
+      <c r="E161" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
-      <c r="B162">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
+        <v>14</v>
+      </c>
+      <c r="C162">
+        <v>100</v>
+      </c>
+      <c r="D162">
+        <v>100</v>
+      </c>
+      <c r="E162" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
-      <c r="B163">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>14</v>
+      </c>
+      <c r="C163">
+        <v>100</v>
+      </c>
+      <c r="D163">
+        <v>100</v>
+      </c>
+      <c r="E163" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
-      <c r="B164">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>14</v>
+      </c>
+      <c r="C164">
+        <v>100</v>
+      </c>
+      <c r="D164">
+        <v>100</v>
+      </c>
+      <c r="E164" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
-      <c r="B165">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>14</v>
+      </c>
+      <c r="C165">
+        <v>100</v>
+      </c>
+      <c r="D165">
+        <v>100</v>
+      </c>
+      <c r="E165" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
-      <c r="B166">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B166" t="s">
+        <v>14</v>
+      </c>
+      <c r="C166">
+        <v>100</v>
+      </c>
+      <c r="D166">
+        <v>100</v>
+      </c>
+      <c r="E166" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
-      <c r="B167">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
+        <v>14</v>
+      </c>
+      <c r="C167">
+        <v>20</v>
+      </c>
+      <c r="D167">
+        <v>20</v>
+      </c>
+      <c r="E167" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
-      <c r="B168">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B168" t="s">
+        <v>14</v>
+      </c>
+      <c r="C168">
+        <v>20</v>
+      </c>
+      <c r="D168">
+        <v>20</v>
+      </c>
+      <c r="E168" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
-      <c r="B169">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B169" t="s">
+        <v>14</v>
+      </c>
+      <c r="C169">
+        <v>20</v>
+      </c>
+      <c r="D169">
+        <v>20</v>
+      </c>
+      <c r="E169" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
-      <c r="B170">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
+        <v>14</v>
+      </c>
+      <c r="C170">
+        <v>20</v>
+      </c>
+      <c r="D170">
+        <v>20</v>
+      </c>
+      <c r="E170" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
-      <c r="B171">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>14</v>
+      </c>
+      <c r="C171">
+        <v>20</v>
+      </c>
+      <c r="D171">
+        <v>20</v>
+      </c>
+      <c r="E171" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
-      <c r="B172">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
+        <v>14</v>
+      </c>
+      <c r="C172">
+        <v>50</v>
+      </c>
+      <c r="D172">
+        <v>50</v>
+      </c>
+      <c r="E172" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
-      <c r="B173">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
+        <v>14</v>
+      </c>
+      <c r="C173">
+        <v>50</v>
+      </c>
+      <c r="D173">
+        <v>50</v>
+      </c>
+      <c r="E173" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
-      <c r="B174">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
+        <v>14</v>
+      </c>
+      <c r="C174">
+        <v>50</v>
+      </c>
+      <c r="D174">
+        <v>50</v>
+      </c>
+      <c r="E174" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
-      <c r="B175">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B175" t="s">
+        <v>14</v>
+      </c>
+      <c r="C175">
+        <v>50</v>
+      </c>
+      <c r="D175">
+        <v>50</v>
+      </c>
+      <c r="E175" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
-      <c r="B176">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
+        <v>14</v>
+      </c>
+      <c r="C176">
+        <v>50</v>
+      </c>
+      <c r="D176">
+        <v>50</v>
+      </c>
+      <c r="E176" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
-      <c r="B177">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B177" t="s">
+        <v>14</v>
+      </c>
+      <c r="C177">
+        <v>100</v>
+      </c>
+      <c r="D177">
+        <v>100</v>
+      </c>
+      <c r="E177" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
-      <c r="B178">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B178" t="s">
+        <v>14</v>
+      </c>
+      <c r="C178">
+        <v>100</v>
+      </c>
+      <c r="D178">
+        <v>100</v>
+      </c>
+      <c r="E178" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
-      <c r="B179">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B179" t="s">
+        <v>14</v>
+      </c>
+      <c r="C179">
+        <v>100</v>
+      </c>
+      <c r="D179">
+        <v>100</v>
+      </c>
+      <c r="E179" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
-      <c r="B180">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B180" t="s">
+        <v>14</v>
+      </c>
+      <c r="C180">
+        <v>100</v>
+      </c>
+      <c r="D180">
+        <v>100</v>
+      </c>
+      <c r="E180" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
-      <c r="B181">
-        <v>100</v>
+      <c r="B181" t="s">
+        <v>14</v>
+      </c>
+      <c r="C181">
+        <v>100</v>
+      </c>
+      <c r="D181">
+        <v>100</v>
+      </c>
+      <c r="E181" s="7" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1910,7 +3561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>

</xml_diff>